<commit_message>
Sistema de registro completo - nunca mas se pierde historial
- historial_enviados.csv: 607 emails exportados desde IMAP
- exportar_historial_imap.py: exporta historial cuando se necesite
- informe_pendientes.py: genera informe de municipios sin enviar
- scrapear_emails_pendientes.py: scraper para segunda vuelta
- sincronizar_excel_imap.py: sincroniza Excel con IMAP
- .gitignore: ahora guarda archivos de registro importantes
- PENDIENTES.md: 205 municipios para scraping

Estado actual: 607 enviados (Toledo, Cuenca, Ciudad_Real, Almeria, Cadiz, Albacete)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/datos/Espana_Maestro_Completo.xlsx
+++ b/datos/Espana_Maestro_Completo.xlsx
@@ -2491,7 +2491,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/villaverde-de-guadalimar</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:18</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2521,7 +2525,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/casas-de-juan-nunez</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:21</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2551,7 +2559,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/abengibre</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:25</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2581,7 +2593,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/alatoz</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr"/>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:28</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2611,7 +2627,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/albacete</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:31</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2641,7 +2661,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/albatana</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:34</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2671,7 +2695,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/alborea</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:37</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2701,7 +2729,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/alcadozo</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:40</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2731,7 +2763,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/alcala-del-jucar</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:43</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2761,7 +2797,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/alcaraz</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:46</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2791,7 +2831,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/almansa</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr"/>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:49</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2821,7 +2865,11 @@
           <t>https://www.todoslosayuntamientos.es/castilla-la-mancha/albacete/alpera</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2026-01-28 09:52</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">

</xml_diff>